<commit_message>
Improve the login process & remove gateway server
</commit_message>
<xml_diff>
--- a/resource/excel/server/DB.xlsx
+++ b/resource/excel/server/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24600" windowHeight="11315"/>
+    <workbookView windowWidth="28800" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -79,16 +79,13 @@
     <t>pwnsky_squick</t>
   </si>
   <si>
+    <t>MongoPlayerDb_1</t>
+  </si>
+  <si>
     <t>RedisGameDb_1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>MongoPlayerDb_1</t>
   </si>
 </sst>
 </file>
@@ -1228,18 +1225,18 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="24.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="22.1296296296296" customWidth="1"/>
-    <col min="3" max="3" width="35.6296296296296" customWidth="1"/>
+    <col min="2" max="2" width="22.1333333333333" customWidth="1"/>
+    <col min="3" max="3" width="35.6333333333333" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="33.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="24.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="32.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="24.5583333333333" customWidth="1"/>
+    <col min="7" max="7" width="32.5583333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1449,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" ht="15.15" spans="1:7">
+    <row r="10" ht="14.25" spans="1:7">
       <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
@@ -1479,53 +1476,53 @@
         <v>19</v>
       </c>
       <c r="F11" s="15">
-        <v>10100</v>
+        <v>10400</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>23</v>
+      <c r="B12" s="15">
+        <v>2</v>
+      </c>
+      <c r="C12" s="15">
+        <v>2</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="17">
-        <v>10200</v>
+      <c r="F12" s="15">
+        <v>10410</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="15">
-        <v>3</v>
-      </c>
-      <c r="C13" s="15">
-        <v>2</v>
+      <c r="A13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="15">
-        <v>10300</v>
+      <c r="F13" s="17">
+        <v>10420</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>20</v>

</xml_diff>